<commit_message>
updated severity for parameters
</commit_message>
<xml_diff>
--- a/framework/Product Research/ProductResearchTemplate_V1.1.xlsx
+++ b/framework/Product Research/ProductResearchTemplate_V1.1.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +654,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F8" s="5">
         <f>D8*C8</f>
@@ -673,7 +673,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F9" s="5">
         <f>D9*C9</f>

</xml_diff>